<commit_message>
Some bugs in Rospotrebnadzon parsing code
</commit_message>
<xml_diff>
--- a/data/CovidMoscow.xlsx
+++ b/data/CovidMoscow.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>date</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
   </si>
 </sst>
 </file>
@@ -1764,16 +1767,16 @@
         <v>87</v>
       </c>
       <c r="B85" t="n" s="2">
-        <v>43979.0</v>
+        <v>43978.0</v>
       </c>
       <c r="C85" t="n">
-        <v>2054.0</v>
+        <v>2140.0</v>
       </c>
       <c r="D85" t="n">
-        <v>171363.0</v>
+        <v>171449.0</v>
       </c>
       <c r="E85" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="86">
@@ -1781,16 +1784,33 @@
         <v>88</v>
       </c>
       <c r="B86" t="n" s="2">
-        <v>43978.0</v>
+        <v>43979.0</v>
       </c>
       <c r="C86" t="n">
-        <v>2140.0</v>
+        <v>2054.0</v>
       </c>
       <c r="D86" t="n">
         <v>173503.0</v>
       </c>
       <c r="E86" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87" t="n" s="2">
+        <v>43980.0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>2332.0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>175835.0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data update & minor bug
</commit_message>
<xml_diff>
--- a/data/CovidMoscow.xlsx
+++ b/data/CovidMoscow.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>date</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
   </si>
 </sst>
 </file>
@@ -1833,6 +1836,23 @@
         <v>7.0</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" t="n" s="2">
+        <v>43982.0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>2595.0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>180797.0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
data update + shorter span in smooths
</commit_message>
<xml_diff>
--- a/data/CovidMoscow.xlsx
+++ b/data/CovidMoscow.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>date</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
   </si>
 </sst>
 </file>
@@ -1853,6 +1859,40 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" t="n" s="2">
+        <v>43984.0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>2286.0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>183083.0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" t="n" s="2">
+        <v>43983.0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>2297.0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>185380.0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>